<commit_message>
update .xlsx and .py
1. '다중 꺾은 선 그래프' 생성 코드 모듈화
2. 첫번째 팝업으로 .xlsx파일을 선택하고,
두번째 팝업으로 출력할 결과 .html 파일의
이름과 경로를 지정하도록 최적화
3. (한반도 위기론을 배경으로) 미사일, 위성을 검색했을 때
집계되는 뉴스 기사 수를 주 단위로 나타낸 .xlsx 파일 추가

집계 기간: 2013-02-23 ~ 2024-04-06
(각 시작일과 종료일은 토요일에 해당한다.)
따라서 집계되는 주는: '토요일에서 격주 금요일까지'를 반영한다.

지금 돌이켜보면, 종료일은 2024-04-05 (금요일)를 날짜로 지정하는 것이 맞을 것이고
주 단위로 해석하는 그래프를 보는데 있어서

2024-03-30 일로 시작되고, '2024-04-06' 일로
끝나는 데이터 변화는 무시하고 보는 것이 데이터 집계 기간과
주 단위로 나타낸 그래프에 있어서 적절한 선택일 것이다.

조만간 수정해야겠다.
</commit_message>
<xml_diff>
--- a/src/chart-politics/!정치-여당.xlsx
+++ b/src/chart-politics/!정치-여당.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DataScience\[Git-Duckfin] Selection2024\src\chart-politics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E8A10-C0B6-4E52-B7C0-9186D429876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB0169B-1426-409E-A144-7E829A54DA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="3285" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>date</t>
   </si>
@@ -681,15 +681,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048575"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,20 +717,17 @@
       <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>103</v>
+      <c r="I1" t="s">
+        <v>104</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -752,20 +752,17 @@
       <c r="H2" s="1">
         <v>311</v>
       </c>
-      <c r="I2" s="1">
-        <v>311</v>
+      <c r="I2">
+        <v>13</v>
       </c>
       <c r="J2">
-        <v>13</v>
-      </c>
-      <c r="K2">
         <v>7</v>
       </c>
-      <c r="L2" s="1">
+      <c r="K2" s="1">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -790,20 +787,17 @@
       <c r="H3" s="1">
         <v>378</v>
       </c>
-      <c r="I3" s="1">
-        <v>378</v>
+      <c r="I3">
+        <v>28</v>
       </c>
       <c r="J3">
-        <v>28</v>
-      </c>
-      <c r="K3">
         <v>15</v>
       </c>
-      <c r="L3" s="1">
+      <c r="K3" s="1">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -828,20 +822,17 @@
       <c r="H4" s="1">
         <v>279</v>
       </c>
-      <c r="I4" s="1">
-        <v>279</v>
+      <c r="I4">
+        <v>38</v>
       </c>
       <c r="J4">
-        <v>38</v>
-      </c>
-      <c r="K4">
         <v>20</v>
       </c>
-      <c r="L4" s="1">
+      <c r="K4" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -866,20 +857,17 @@
       <c r="H5" s="1">
         <v>244</v>
       </c>
-      <c r="I5" s="1">
-        <v>244</v>
+      <c r="I5">
+        <v>36</v>
       </c>
       <c r="J5">
-        <v>36</v>
-      </c>
-      <c r="K5">
         <v>5</v>
       </c>
-      <c r="L5" s="1">
+      <c r="K5" s="1">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -904,20 +892,17 @@
       <c r="H6" s="1">
         <v>194</v>
       </c>
-      <c r="I6" s="1">
-        <v>194</v>
+      <c r="I6">
+        <v>20</v>
       </c>
       <c r="J6">
-        <v>20</v>
-      </c>
-      <c r="K6">
         <v>10</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K6" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,20 +927,17 @@
       <c r="H7" s="1">
         <v>772</v>
       </c>
-      <c r="I7" s="1">
-        <v>772</v>
+      <c r="I7">
+        <v>11</v>
       </c>
       <c r="J7">
-        <v>11</v>
-      </c>
-      <c r="K7">
         <v>6</v>
       </c>
-      <c r="L7" s="1">
+      <c r="K7" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -980,20 +962,17 @@
       <c r="H8" s="1">
         <v>395</v>
       </c>
-      <c r="I8" s="1">
-        <v>395</v>
+      <c r="I8">
+        <v>3</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="K8" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,20 +997,17 @@
       <c r="H9" s="1">
         <v>255</v>
       </c>
-      <c r="I9" s="1">
-        <v>255</v>
+      <c r="I9">
+        <v>21</v>
       </c>
       <c r="J9">
-        <v>21</v>
-      </c>
-      <c r="K9">
         <v>9</v>
       </c>
-      <c r="L9" s="1">
+      <c r="K9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1056,20 +1032,17 @@
       <c r="H10" s="1">
         <v>1124</v>
       </c>
-      <c r="I10" s="1">
-        <v>1124</v>
+      <c r="I10">
+        <v>12</v>
       </c>
       <c r="J10">
-        <v>12</v>
-      </c>
-      <c r="K10">
         <v>7</v>
       </c>
-      <c r="L10" s="1">
+      <c r="K10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1094,20 +1067,17 @@
       <c r="H11" s="1">
         <v>492</v>
       </c>
-      <c r="I11" s="1">
-        <v>492</v>
+      <c r="I11">
+        <v>7</v>
       </c>
       <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="K11">
         <v>5</v>
       </c>
-      <c r="L11" s="1">
+      <c r="K11" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1132,20 +1102,17 @@
       <c r="H12" s="1">
         <v>495</v>
       </c>
-      <c r="I12" s="1">
-        <v>495</v>
+      <c r="I12">
+        <v>32</v>
       </c>
       <c r="J12">
-        <v>32</v>
-      </c>
-      <c r="K12">
         <v>7</v>
       </c>
-      <c r="L12" s="1">
+      <c r="K12" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1170,20 +1137,17 @@
       <c r="H13" s="1">
         <v>277</v>
       </c>
-      <c r="I13" s="1">
-        <v>277</v>
+      <c r="I13">
+        <v>17</v>
       </c>
       <c r="J13">
-        <v>17</v>
-      </c>
-      <c r="K13">
         <v>8</v>
       </c>
-      <c r="L13" s="1">
+      <c r="K13" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1208,20 +1172,17 @@
       <c r="H14" s="1">
         <v>810</v>
       </c>
-      <c r="I14" s="1">
-        <v>810</v>
+      <c r="I14">
+        <v>20</v>
       </c>
       <c r="J14">
-        <v>20</v>
-      </c>
-      <c r="K14">
         <v>10</v>
       </c>
-      <c r="L14" s="1">
+      <c r="K14" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1246,20 +1207,17 @@
       <c r="H15" s="1">
         <v>463</v>
       </c>
-      <c r="I15" s="1">
-        <v>463</v>
+      <c r="I15">
+        <v>17</v>
       </c>
       <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15" s="1">
         <v>17</v>
       </c>
-      <c r="K15">
-        <v>13</v>
-      </c>
-      <c r="L15" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1284,20 +1242,17 @@
       <c r="H16" s="1">
         <v>313</v>
       </c>
-      <c r="I16" s="1">
-        <v>313</v>
+      <c r="I16">
+        <v>12</v>
       </c>
       <c r="J16">
         <v>12</v>
       </c>
-      <c r="K16">
-        <v>12</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="K16" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1322,20 +1277,17 @@
       <c r="H17" s="1">
         <v>259</v>
       </c>
-      <c r="I17" s="1">
-        <v>259</v>
+      <c r="I17">
+        <v>8</v>
       </c>
       <c r="J17">
         <v>8</v>
       </c>
-      <c r="K17">
-        <v>8</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="K17" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1360,20 +1312,17 @@
       <c r="H18" s="1">
         <v>45</v>
       </c>
-      <c r="I18" s="1">
-        <v>45</v>
+      <c r="I18">
+        <v>12</v>
       </c>
       <c r="J18">
-        <v>12</v>
-      </c>
-      <c r="K18">
         <v>10</v>
       </c>
-      <c r="L18" s="1">
+      <c r="K18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1398,20 +1347,17 @@
       <c r="H19" s="1">
         <v>82</v>
       </c>
-      <c r="I19" s="1">
-        <v>82</v>
+      <c r="I19">
+        <v>6</v>
       </c>
       <c r="J19">
-        <v>6</v>
-      </c>
-      <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1436,20 +1382,17 @@
       <c r="H20" s="1">
         <v>120</v>
       </c>
-      <c r="I20" s="1">
-        <v>120</v>
+      <c r="I20">
+        <v>7</v>
       </c>
       <c r="J20">
         <v>7</v>
       </c>
-      <c r="K20">
-        <v>7</v>
-      </c>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1474,20 +1417,17 @@
       <c r="H21" s="1">
         <v>21</v>
       </c>
-      <c r="I21" s="1">
-        <v>21</v>
+      <c r="I21">
+        <v>7</v>
       </c>
       <c r="J21">
         <v>7</v>
       </c>
-      <c r="K21">
-        <v>7</v>
-      </c>
-      <c r="L21" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1512,20 +1452,17 @@
       <c r="H22" s="1">
         <v>12</v>
       </c>
-      <c r="I22" s="1">
-        <v>12</v>
+      <c r="I22">
+        <v>29</v>
       </c>
       <c r="J22">
-        <v>29</v>
-      </c>
-      <c r="K22">
         <v>27</v>
       </c>
-      <c r="L22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1550,20 +1487,17 @@
       <c r="H23" s="1">
         <v>8</v>
       </c>
-      <c r="I23" s="1">
-        <v>8</v>
+      <c r="I23">
+        <v>27</v>
       </c>
       <c r="J23">
-        <v>27</v>
-      </c>
-      <c r="K23">
         <v>15</v>
       </c>
-      <c r="L23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1588,20 +1522,17 @@
       <c r="H24" s="1">
         <v>2</v>
       </c>
-      <c r="I24" s="1">
-        <v>2</v>
+      <c r="I24">
+        <v>11</v>
       </c>
       <c r="J24">
         <v>11</v>
       </c>
-      <c r="K24">
-        <v>11</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1626,20 +1557,17 @@
       <c r="H25" s="1">
         <v>16</v>
       </c>
-      <c r="I25" s="1">
-        <v>16</v>
+      <c r="I25">
+        <v>4</v>
       </c>
       <c r="J25">
         <v>4</v>
       </c>
-      <c r="K25">
-        <v>4</v>
-      </c>
-      <c r="L25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1664,20 +1592,17 @@
       <c r="H26" s="1">
         <v>7</v>
       </c>
-      <c r="I26" s="1">
-        <v>7</v>
+      <c r="I26">
+        <v>15</v>
       </c>
       <c r="J26">
-        <v>15</v>
-      </c>
-      <c r="K26">
         <v>8</v>
       </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1702,20 +1627,17 @@
       <c r="H27" s="1">
         <v>32</v>
       </c>
-      <c r="I27" s="1">
-        <v>32</v>
+      <c r="I27">
+        <v>18</v>
       </c>
       <c r="J27">
-        <v>18</v>
-      </c>
-      <c r="K27">
         <v>11</v>
       </c>
-      <c r="L27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1740,20 +1662,17 @@
       <c r="H28" s="1">
         <v>17</v>
       </c>
-      <c r="I28" s="1">
-        <v>17</v>
+      <c r="I28">
+        <v>18</v>
       </c>
       <c r="J28">
         <v>18</v>
       </c>
-      <c r="K28">
-        <v>18</v>
-      </c>
-      <c r="L28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1778,20 +1697,17 @@
       <c r="H29" s="1">
         <v>35</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29">
         <v>35</v>
       </c>
       <c r="J29">
-        <v>35</v>
-      </c>
-      <c r="K29">
         <v>34</v>
       </c>
-      <c r="L29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1816,20 +1732,17 @@
       <c r="H30" s="1">
         <v>60</v>
       </c>
-      <c r="I30" s="1">
-        <v>60</v>
+      <c r="I30">
+        <v>3</v>
       </c>
       <c r="J30">
         <v>3</v>
       </c>
-      <c r="K30">
-        <v>3</v>
-      </c>
-      <c r="L30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1854,20 +1767,17 @@
       <c r="H31" s="1">
         <v>41</v>
       </c>
-      <c r="I31" s="1">
-        <v>41</v>
+      <c r="I31">
+        <v>15</v>
       </c>
       <c r="J31">
-        <v>15</v>
-      </c>
-      <c r="K31">
         <v>13</v>
       </c>
-      <c r="L31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1892,20 +1802,17 @@
       <c r="H32" s="1">
         <v>37</v>
       </c>
-      <c r="I32" s="1">
-        <v>37</v>
+      <c r="I32">
+        <v>4</v>
       </c>
       <c r="J32">
-        <v>4</v>
-      </c>
-      <c r="K32">
-        <v>3</v>
-      </c>
-      <c r="L32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1930,20 +1837,17 @@
       <c r="H33" s="1">
         <v>28</v>
       </c>
-      <c r="I33" s="1">
-        <v>28</v>
+      <c r="I33">
+        <v>1</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1968,20 +1872,17 @@
       <c r="H34" s="1">
         <v>10</v>
       </c>
-      <c r="I34" s="1">
-        <v>10</v>
+      <c r="I34">
+        <v>4</v>
       </c>
       <c r="J34">
         <v>4</v>
       </c>
-      <c r="K34">
-        <v>4</v>
-      </c>
-      <c r="L34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -2006,20 +1907,17 @@
       <c r="H35" s="1">
         <v>14</v>
       </c>
-      <c r="I35" s="1">
-        <v>14</v>
+      <c r="I35">
+        <v>1</v>
       </c>
       <c r="J35">
         <v>1</v>
       </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -2044,20 +1942,17 @@
       <c r="H36" s="1">
         <v>33</v>
       </c>
-      <c r="I36" s="1">
-        <v>33</v>
+      <c r="I36">
+        <v>2</v>
       </c>
       <c r="J36">
         <v>2</v>
       </c>
-      <c r="K36">
-        <v>2</v>
-      </c>
-      <c r="L36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -2082,20 +1977,17 @@
       <c r="H37" s="1">
         <v>20</v>
       </c>
-      <c r="I37" s="1">
-        <v>20</v>
+      <c r="I37">
+        <v>6</v>
       </c>
       <c r="J37">
         <v>6</v>
       </c>
-      <c r="K37">
-        <v>6</v>
-      </c>
-      <c r="L37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -2120,20 +2012,17 @@
       <c r="H38" s="1">
         <v>7</v>
       </c>
-      <c r="I38" s="1">
-        <v>7</v>
+      <c r="I38">
+        <v>3</v>
       </c>
       <c r="J38">
-        <v>3</v>
-      </c>
-      <c r="K38">
-        <v>2</v>
-      </c>
-      <c r="L38" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2158,20 +2047,17 @@
       <c r="H39" s="1">
         <v>13</v>
       </c>
-      <c r="I39" s="1">
-        <v>13</v>
+      <c r="I39">
+        <v>12</v>
       </c>
       <c r="J39">
-        <v>12</v>
-      </c>
-      <c r="K39">
         <v>9</v>
       </c>
-      <c r="L39" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -2196,20 +2082,17 @@
       <c r="H40" s="1">
         <v>11</v>
       </c>
-      <c r="I40" s="1">
-        <v>11</v>
+      <c r="I40">
+        <v>14</v>
       </c>
       <c r="J40">
-        <v>14</v>
-      </c>
-      <c r="K40">
         <v>10</v>
       </c>
-      <c r="L40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -2234,20 +2117,17 @@
       <c r="H41" s="1">
         <v>15</v>
       </c>
-      <c r="I41" s="1">
-        <v>15</v>
+      <c r="I41">
+        <v>3</v>
       </c>
       <c r="J41">
-        <v>3</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -2272,20 +2152,17 @@
       <c r="H42" s="1">
         <v>19</v>
       </c>
-      <c r="I42" s="1">
-        <v>19</v>
+      <c r="I42">
+        <v>4</v>
       </c>
       <c r="J42">
-        <v>4</v>
-      </c>
-      <c r="K42">
-        <v>3</v>
-      </c>
-      <c r="L42" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="K42" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -2310,20 +2187,17 @@
       <c r="H43" s="1">
         <v>2</v>
       </c>
-      <c r="I43" s="1">
-        <v>2</v>
+      <c r="I43">
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43" s="1">
+      <c r="K43" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -2348,20 +2222,17 @@
       <c r="H44" s="1">
         <v>4</v>
       </c>
-      <c r="I44" s="1">
-        <v>4</v>
+      <c r="I44">
+        <v>5</v>
       </c>
       <c r="J44">
-        <v>5</v>
-      </c>
-      <c r="K44">
-        <v>2</v>
-      </c>
-      <c r="L44" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="K44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -2386,20 +2257,17 @@
       <c r="H45" s="1">
         <v>4</v>
       </c>
-      <c r="I45" s="1">
-        <v>4</v>
+      <c r="I45">
+        <v>2</v>
       </c>
       <c r="J45">
         <v>2</v>
       </c>
-      <c r="K45">
-        <v>2</v>
-      </c>
-      <c r="L45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -2424,20 +2292,17 @@
       <c r="H46" s="1">
         <v>4</v>
       </c>
-      <c r="I46" s="1">
-        <v>4</v>
+      <c r="I46">
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>1</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -2462,20 +2327,17 @@
       <c r="H47" s="1">
         <v>2</v>
       </c>
-      <c r="I47" s="1">
-        <v>2</v>
+      <c r="I47">
+        <v>0</v>
       </c>
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -2500,20 +2362,17 @@
       <c r="H48" s="1">
         <v>2</v>
       </c>
-      <c r="I48" s="1">
-        <v>2</v>
+      <c r="I48">
+        <v>0</v>
       </c>
       <c r="J48">
         <v>0</v>
       </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -2538,20 +2397,17 @@
       <c r="H49" s="1">
         <v>1</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49">
         <v>1</v>
       </c>
       <c r="J49">
-        <v>1</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -2576,20 +2432,17 @@
       <c r="H50" s="1">
         <v>31</v>
       </c>
-      <c r="I50" s="1">
-        <v>31</v>
+      <c r="I50">
+        <v>2</v>
       </c>
       <c r="J50">
-        <v>2</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -2614,20 +2467,17 @@
       <c r="H51" s="1">
         <v>9</v>
       </c>
-      <c r="I51" s="1">
-        <v>9</v>
+      <c r="I51">
+        <v>3</v>
       </c>
       <c r="J51">
-        <v>3</v>
-      </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
-      <c r="L51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -2652,20 +2502,17 @@
       <c r="H52" s="1">
         <v>3</v>
       </c>
-      <c r="I52" s="1">
-        <v>3</v>
+      <c r="I52">
+        <v>5</v>
       </c>
       <c r="J52">
-        <v>5</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -2690,20 +2537,17 @@
       <c r="H53" s="1">
         <v>1</v>
       </c>
-      <c r="I53" s="1">
-        <v>1</v>
+      <c r="I53">
+        <v>0</v>
       </c>
       <c r="J53">
         <v>0</v>
       </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
@@ -2728,20 +2572,17 @@
       <c r="H54" s="1">
         <v>7</v>
       </c>
-      <c r="I54" s="1">
-        <v>7</v>
+      <c r="I54">
+        <v>2</v>
       </c>
       <c r="J54">
-        <v>2</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54" s="1">
+        <v>1</v>
+      </c>
+      <c r="K54" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -2766,20 +2607,17 @@
       <c r="H55" s="1">
         <v>1</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55">
         <v>1</v>
       </c>
       <c r="J55">
         <v>1</v>
       </c>
-      <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K55" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -2804,20 +2642,17 @@
       <c r="H56" s="1">
         <v>0</v>
       </c>
-      <c r="I56" s="1">
-        <v>0</v>
+      <c r="I56">
+        <v>2</v>
       </c>
       <c r="J56">
-        <v>2</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -2842,20 +2677,17 @@
       <c r="H57" s="1">
         <v>1</v>
       </c>
-      <c r="I57" s="1">
-        <v>1</v>
+      <c r="I57">
+        <v>4</v>
       </c>
       <c r="J57">
-        <v>4</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
@@ -2880,20 +2712,17 @@
       <c r="H58" s="1">
         <v>0</v>
       </c>
-      <c r="I58" s="1">
-        <v>0</v>
+      <c r="I58">
+        <v>1</v>
       </c>
       <c r="J58">
         <v>1</v>
       </c>
-      <c r="K58">
-        <v>1</v>
-      </c>
-      <c r="L58" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
@@ -2918,20 +2747,17 @@
       <c r="H59" s="1">
         <v>1</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59">
         <v>1</v>
       </c>
       <c r="J59">
         <v>1</v>
       </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -2956,20 +2782,17 @@
       <c r="H60" s="1">
         <v>2</v>
       </c>
-      <c r="I60" s="1">
-        <v>2</v>
+      <c r="I60">
+        <v>0</v>
       </c>
       <c r="J60">
         <v>0</v>
       </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
@@ -2994,20 +2817,17 @@
       <c r="H61" s="1">
         <v>1</v>
       </c>
-      <c r="I61" s="1">
-        <v>1</v>
+      <c r="I61">
+        <v>0</v>
       </c>
       <c r="J61">
         <v>0</v>
       </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61" s="1">
+      <c r="K61" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
@@ -3032,20 +2852,17 @@
       <c r="H62" s="1">
         <v>1</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62">
         <v>1</v>
       </c>
       <c r="J62">
         <v>1</v>
       </c>
-      <c r="K62">
-        <v>1</v>
-      </c>
-      <c r="L62" s="1">
+      <c r="K62" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
@@ -3070,20 +2887,17 @@
       <c r="H63" s="1">
         <v>1</v>
       </c>
-      <c r="I63" s="1">
-        <v>1</v>
+      <c r="I63">
+        <v>0</v>
       </c>
       <c r="J63">
         <v>0</v>
       </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63" s="1">
+      <c r="K63" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -3108,20 +2922,17 @@
       <c r="H64" s="1">
         <v>5</v>
       </c>
-      <c r="I64" s="1">
-        <v>5</v>
+      <c r="I64">
+        <v>1</v>
       </c>
       <c r="J64">
         <v>1</v>
       </c>
-      <c r="K64">
-        <v>1</v>
-      </c>
-      <c r="L64" s="1">
+      <c r="K64" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -3146,20 +2957,17 @@
       <c r="H65" s="1">
         <v>23</v>
       </c>
-      <c r="I65" s="1">
-        <v>23</v>
+      <c r="I65">
+        <v>1</v>
       </c>
       <c r="J65">
         <v>1</v>
       </c>
-      <c r="K65">
-        <v>1</v>
-      </c>
-      <c r="L65" s="1">
+      <c r="K65" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
@@ -3184,20 +2992,17 @@
       <c r="H66" s="1">
         <v>0</v>
       </c>
-      <c r="I66" s="1">
-        <v>0</v>
+      <c r="I66">
+        <v>6</v>
       </c>
       <c r="J66">
-        <v>6</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
@@ -3222,20 +3027,17 @@
       <c r="H67" s="1">
         <v>0</v>
       </c>
-      <c r="I67" s="1">
-        <v>0</v>
+      <c r="I67">
+        <v>7</v>
       </c>
       <c r="J67">
-        <v>7</v>
-      </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
@@ -3260,20 +3062,17 @@
       <c r="H68" s="1">
         <v>1</v>
       </c>
-      <c r="I68" s="1">
+      <c r="I68">
         <v>1</v>
       </c>
       <c r="J68">
-        <v>1</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
@@ -3298,20 +3097,17 @@
       <c r="H69" s="1">
         <v>1</v>
       </c>
-      <c r="I69" s="1">
-        <v>1</v>
+      <c r="I69">
+        <v>4</v>
       </c>
       <c r="J69">
-        <v>4</v>
-      </c>
-      <c r="K69">
-        <v>1</v>
-      </c>
-      <c r="L69" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
@@ -3336,20 +3132,17 @@
       <c r="H70" s="1">
         <v>2</v>
       </c>
-      <c r="I70" s="1">
-        <v>2</v>
+      <c r="I70">
+        <v>6</v>
       </c>
       <c r="J70">
-        <v>6</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
@@ -3374,20 +3167,17 @@
       <c r="H71" s="1">
         <v>0</v>
       </c>
-      <c r="I71" s="1">
-        <v>0</v>
+      <c r="I71">
+        <v>4</v>
       </c>
       <c r="J71">
-        <v>4</v>
-      </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
-      <c r="L71" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
@@ -3412,20 +3202,17 @@
       <c r="H72" s="1">
         <v>1</v>
       </c>
-      <c r="I72" s="1">
-        <v>1</v>
+      <c r="I72">
+        <v>8</v>
       </c>
       <c r="J72">
-        <v>8</v>
-      </c>
-      <c r="K72">
-        <v>1</v>
-      </c>
-      <c r="L72" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
@@ -3450,20 +3237,17 @@
       <c r="H73" s="1">
         <v>4</v>
       </c>
-      <c r="I73" s="1">
-        <v>4</v>
+      <c r="I73">
+        <v>3</v>
       </c>
       <c r="J73">
-        <v>3</v>
-      </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
-      <c r="L73" s="1">
+        <v>1</v>
+      </c>
+      <c r="K73" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
@@ -3488,20 +3272,17 @@
       <c r="H74" s="1">
         <v>2</v>
       </c>
-      <c r="I74" s="1">
-        <v>2</v>
+      <c r="I74">
+        <v>7</v>
       </c>
       <c r="J74">
-        <v>7</v>
-      </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="L74" s="1">
+        <v>1</v>
+      </c>
+      <c r="K74" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
@@ -3526,20 +3307,17 @@
       <c r="H75" s="1">
         <v>4</v>
       </c>
-      <c r="I75" s="1">
-        <v>4</v>
+      <c r="I75">
+        <v>2</v>
       </c>
       <c r="J75">
-        <v>2</v>
-      </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-      <c r="L75" s="1">
+        <v>0</v>
+      </c>
+      <c r="K75" s="1">
         <v>377</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>76</v>
       </c>
@@ -3564,20 +3342,17 @@
       <c r="H76" s="1">
         <v>35</v>
       </c>
-      <c r="I76" s="1">
-        <v>35</v>
+      <c r="I76">
+        <v>4</v>
       </c>
       <c r="J76">
-        <v>4</v>
-      </c>
-      <c r="K76">
-        <v>3</v>
-      </c>
-      <c r="L76" s="1">
+        <v>3</v>
+      </c>
+      <c r="K76" s="1">
         <v>382</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
@@ -3602,20 +3377,17 @@
       <c r="H77" s="1">
         <v>18</v>
       </c>
-      <c r="I77" s="1">
-        <v>18</v>
+      <c r="I77">
+        <v>14</v>
       </c>
       <c r="J77">
-        <v>14</v>
-      </c>
-      <c r="K77">
-        <v>2</v>
-      </c>
-      <c r="L77" s="1">
+        <v>2</v>
+      </c>
+      <c r="K77" s="1">
         <v>241</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
@@ -3640,20 +3412,17 @@
       <c r="H78" s="1">
         <v>12</v>
       </c>
-      <c r="I78" s="1">
-        <v>12</v>
+      <c r="I78">
+        <v>76</v>
       </c>
       <c r="J78">
-        <v>76</v>
-      </c>
-      <c r="K78">
         <v>20</v>
       </c>
-      <c r="L78" s="1">
+      <c r="K78" s="1">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
@@ -3678,20 +3447,17 @@
       <c r="H79" s="1">
         <v>1</v>
       </c>
-      <c r="I79" s="1">
-        <v>1</v>
+      <c r="I79">
+        <v>27</v>
       </c>
       <c r="J79">
-        <v>27</v>
-      </c>
-      <c r="K79">
-        <v>2</v>
-      </c>
-      <c r="L79" s="1">
+        <v>2</v>
+      </c>
+      <c r="K79" s="1">
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
@@ -3716,20 +3482,17 @@
       <c r="H80" s="1">
         <v>1</v>
       </c>
-      <c r="I80" s="1">
-        <v>1</v>
+      <c r="I80">
+        <v>24</v>
       </c>
       <c r="J80">
-        <v>24</v>
-      </c>
-      <c r="K80">
         <v>5</v>
       </c>
-      <c r="L80" s="1">
+      <c r="K80" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
@@ -3754,20 +3517,17 @@
       <c r="H81" s="1">
         <v>12</v>
       </c>
-      <c r="I81" s="1">
-        <v>12</v>
+      <c r="I81">
+        <v>11</v>
       </c>
       <c r="J81">
-        <v>11</v>
-      </c>
-      <c r="K81">
-        <v>4</v>
-      </c>
-      <c r="L81" s="1">
+        <v>4</v>
+      </c>
+      <c r="K81" s="1">
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
@@ -3792,20 +3552,17 @@
       <c r="H82" s="1">
         <v>44</v>
       </c>
-      <c r="I82" s="1">
-        <v>44</v>
+      <c r="I82">
+        <v>592</v>
       </c>
       <c r="J82">
-        <v>592</v>
-      </c>
-      <c r="K82">
         <v>159</v>
       </c>
-      <c r="L82" s="1">
+      <c r="K82" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>83</v>
       </c>
@@ -3830,20 +3587,17 @@
       <c r="H83" s="1">
         <v>3</v>
       </c>
-      <c r="I83" s="1">
-        <v>3</v>
+      <c r="I83">
+        <v>947</v>
       </c>
       <c r="J83">
-        <v>947</v>
-      </c>
-      <c r="K83">
         <v>43</v>
       </c>
-      <c r="L83" s="1">
+      <c r="K83" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
@@ -3868,20 +3622,17 @@
       <c r="H84" s="1">
         <v>3</v>
       </c>
-      <c r="I84" s="1">
-        <v>3</v>
+      <c r="I84">
+        <v>789</v>
       </c>
       <c r="J84">
-        <v>789</v>
-      </c>
-      <c r="K84">
         <v>32</v>
       </c>
-      <c r="L84" s="1">
+      <c r="K84" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
@@ -3906,20 +3657,17 @@
       <c r="H85" s="1">
         <v>2</v>
       </c>
-      <c r="I85" s="1">
-        <v>2</v>
+      <c r="I85">
+        <v>471</v>
       </c>
       <c r="J85">
-        <v>471</v>
-      </c>
-      <c r="K85">
         <v>49</v>
       </c>
-      <c r="L85" s="1">
+      <c r="K85" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
@@ -3944,20 +3692,17 @@
       <c r="H86" s="1">
         <v>12</v>
       </c>
-      <c r="I86" s="1">
-        <v>12</v>
+      <c r="I86">
+        <v>386</v>
       </c>
       <c r="J86">
-        <v>386</v>
-      </c>
-      <c r="K86">
         <v>73</v>
       </c>
-      <c r="L86" s="1">
+      <c r="K86" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
@@ -3982,20 +3727,17 @@
       <c r="H87" s="1">
         <v>40</v>
       </c>
-      <c r="I87" s="1">
-        <v>40</v>
+      <c r="I87">
+        <v>688</v>
       </c>
       <c r="J87">
-        <v>688</v>
-      </c>
-      <c r="K87">
         <v>68</v>
       </c>
-      <c r="L87" s="1">
+      <c r="K87" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
@@ -4020,20 +3762,17 @@
       <c r="H88" s="1">
         <v>15</v>
       </c>
-      <c r="I88" s="1">
-        <v>15</v>
+      <c r="I88">
+        <v>466</v>
       </c>
       <c r="J88">
-        <v>466</v>
-      </c>
-      <c r="K88">
         <v>31</v>
       </c>
-      <c r="L88" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
@@ -4058,20 +3797,17 @@
       <c r="H89" s="1">
         <v>0</v>
       </c>
-      <c r="I89" s="1">
-        <v>0</v>
+      <c r="I89">
+        <v>333</v>
       </c>
       <c r="J89">
-        <v>333</v>
-      </c>
-      <c r="K89">
         <v>23</v>
       </c>
-      <c r="L89" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K89" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
@@ -4096,20 +3832,17 @@
       <c r="H90" s="1">
         <v>1</v>
       </c>
-      <c r="I90" s="1">
-        <v>1</v>
+      <c r="I90">
+        <v>260</v>
       </c>
       <c r="J90">
-        <v>260</v>
-      </c>
-      <c r="K90">
         <v>17</v>
       </c>
-      <c r="L90" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K90" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>91</v>
       </c>
@@ -4134,20 +3867,17 @@
       <c r="H91" s="1">
         <v>4</v>
       </c>
-      <c r="I91" s="1">
-        <v>4</v>
+      <c r="I91">
+        <v>212</v>
       </c>
       <c r="J91">
-        <v>212</v>
-      </c>
-      <c r="K91">
         <v>43</v>
       </c>
-      <c r="L91" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
@@ -4172,20 +3902,17 @@
       <c r="H92" s="1">
         <v>6</v>
       </c>
-      <c r="I92" s="1">
-        <v>6</v>
+      <c r="I92">
+        <v>255</v>
       </c>
       <c r="J92">
-        <v>255</v>
-      </c>
-      <c r="K92">
         <v>55</v>
       </c>
-      <c r="L92" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
@@ -4210,20 +3937,17 @@
       <c r="H93" s="1">
         <v>2</v>
       </c>
-      <c r="I93" s="1">
-        <v>2</v>
+      <c r="I93">
+        <v>208</v>
       </c>
       <c r="J93">
-        <v>208</v>
-      </c>
-      <c r="K93">
         <v>16</v>
       </c>
-      <c r="L93" s="1">
+      <c r="K93" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
@@ -4248,20 +3972,17 @@
       <c r="H94" s="1">
         <v>1</v>
       </c>
-      <c r="I94" s="1">
-        <v>1</v>
+      <c r="I94">
+        <v>308</v>
       </c>
       <c r="J94">
-        <v>308</v>
-      </c>
-      <c r="K94">
         <v>15</v>
       </c>
-      <c r="L94" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K94" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>95</v>
       </c>
@@ -4286,20 +4007,17 @@
       <c r="H95" s="1">
         <v>2</v>
       </c>
-      <c r="I95" s="1">
-        <v>2</v>
+      <c r="I95">
+        <v>286</v>
       </c>
       <c r="J95">
-        <v>286</v>
-      </c>
-      <c r="K95">
         <v>52</v>
       </c>
-      <c r="L95" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K95" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>96</v>
       </c>
@@ -4324,20 +4042,17 @@
       <c r="H96" s="1">
         <v>3</v>
       </c>
-      <c r="I96" s="1">
-        <v>3</v>
+      <c r="I96">
+        <v>337</v>
       </c>
       <c r="J96">
-        <v>337</v>
-      </c>
-      <c r="K96">
         <v>83</v>
       </c>
-      <c r="L96" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>97</v>
       </c>
@@ -4362,16 +4077,13 @@
       <c r="H97" s="1">
         <v>1</v>
       </c>
-      <c r="I97" s="1">
-        <v>1</v>
+      <c r="I97">
+        <v>208</v>
       </c>
       <c r="J97">
-        <v>208</v>
-      </c>
-      <c r="K97">
         <v>14</v>
       </c>
-      <c r="L97" s="1">
+      <c r="K97" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>